<commit_message>
Se comienza a desarrollar liquidaciones de sueldos en lote
</commit_message>
<xml_diff>
--- a/src/Mbp/PersonalBundle/Resources/doc/fichadas.xlsx
+++ b/src/Mbp/PersonalBundle/Resources/doc/fichadas.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14196" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14195" uniqueCount="411">
   <si>
     <t>legajo</t>
   </si>
@@ -1285,9 +1285,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1592,7 +1593,7 @@
   <dimension ref="A1:U676"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,7 +1602,8 @@
     <col min="3" max="3" width="49" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="17" width="5" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="17" width="5" customWidth="1"/>
     <col min="18" max="19" width="6" customWidth="1"/>
     <col min="20" max="20" width="50" customWidth="1"/>
     <col min="21" max="21" width="23" customWidth="1"/>
@@ -1688,8 +1690,8 @@
       <c r="E2" t="s">
         <v>31</v>
       </c>
-      <c r="F2" t="s">
-        <v>32</v>
+      <c r="F2" s="2">
+        <v>0.29166666666666669</v>
       </c>
       <c r="G2" t="s">
         <v>33</v>

</xml_diff>